<commit_message>
CHARMS - RAS Survey Form Verification - Demographics/RASopathy History/Birth & Gestation
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/RASScenario2.xlsx
+++ b/src/test/java/CHARMS/resources/RASScenario2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzipovay2/AquaProjects/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF38096D-B844-B64A-A38B-678CC3141B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434784B0-9A57-5343-8CF9-F3EDE000524E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="screenerScenario2" sheetId="1" r:id="rId1"/>
@@ -9742,7 +9742,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -9806,6 +9806,7 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10125,7 +10126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="108" workbookViewId="0">
+    <sheetView zoomScale="162" zoomScaleNormal="108" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -12836,8 +12837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9D8CBE7-FBBE-194B-88E2-C1DC4C20EF1C}">
   <dimension ref="A1:B1412"/>
   <sheetViews>
-    <sheetView topLeftCell="A378" workbookViewId="0">
-      <selection activeCell="B1372" sqref="B1372"/>
+    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A264" sqref="A264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14042,7 +14043,7 @@
       <c r="A150" s="3" t="s">
         <v>831</v>
       </c>
-      <c r="B150">
+      <c r="B150" s="25">
         <v>600</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CHARMS - RAS Survey Verification in Native View
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/RASScenario2.xlsx
+++ b/src/test/java/CHARMS/resources/RASScenario2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzipovay2/AquaProjects/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434784B0-9A57-5343-8CF9-F3EDE000524E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11885279-AD9F-7541-A6AC-E7A3FEC3FFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="screenerScenario2" sheetId="1" r:id="rId1"/>
@@ -10126,8 +10126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B152"/>
   <sheetViews>
-    <sheetView zoomScale="162" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12837,7 +12837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9D8CBE7-FBBE-194B-88E2-C1DC4C20EF1C}">
   <dimension ref="A1:B1412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A264" sqref="A264"/>
     </sheetView>
   </sheetViews>
@@ -24128,6 +24128,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010084299BAE6AB37648AD80DEB59DC34125" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3eadf2c1f25cd7b71915c87a24a5e490">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="70b45aa3-433c-4bb7-a757-4861a21b7bcd" xmlns:ns3="f9acbf48-ccda-47b6-abb6-c9eb96c9ba33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="383f12c7747b491aea3350ad3b69b32a" ns2:_="" ns3:_="">
     <xsd:import namespace="70b45aa3-433c-4bb7-a757-4861a21b7bcd"/>
@@ -24298,22 +24313,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A376A26F-A459-4EA6-9FC7-DF620BE07CA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B75DB3A7-FCD6-4DD2-8F1A-F1A891316494}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8739BBC0-A319-48B2-92BB-329AC3208E3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24330,21 +24347,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B75DB3A7-FCD6-4DD2-8F1A-F1A891316494}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A376A26F-A459-4EA6-9FC7-DF620BE07CA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
CHARMS - Updated NV scenario code to reflect latest changes
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/RASScenario2.xlsx
+++ b/src/test/java/CHARMS/resources/RASScenario2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzipovay2/AquaProjects/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752275F2-5998-A54C-8405-ABAA09444B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0CB48B-EE94-8744-85CA-B66B2B5102AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="screenerScenario2" sheetId="1" r:id="rId1"/>
@@ -10129,8 +10129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B153"/>
   <sheetViews>
-    <sheetView zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12848,8 +12848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9D8CBE7-FBBE-194B-88E2-C1DC4C20EF1C}">
   <dimension ref="A1:B1412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1367" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A1376" sqref="A1376"/>
+    <sheetView topLeftCell="A1226" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A1326" sqref="A1326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -24139,21 +24139,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010084299BAE6AB37648AD80DEB59DC34125" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3eadf2c1f25cd7b71915c87a24a5e490">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="70b45aa3-433c-4bb7-a757-4861a21b7bcd" xmlns:ns3="f9acbf48-ccda-47b6-abb6-c9eb96c9ba33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="383f12c7747b491aea3350ad3b69b32a" ns2:_="" ns3:_="">
     <xsd:import namespace="70b45aa3-433c-4bb7-a757-4861a21b7bcd"/>
@@ -24324,24 +24309,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A376A26F-A459-4EA6-9FC7-DF620BE07CA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B75DB3A7-FCD6-4DD2-8F1A-F1A891316494}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8739BBC0-A319-48B2-92BB-329AC3208E3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24358,4 +24341,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B75DB3A7-FCD6-4DD2-8F1A-F1A891316494}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A376A26F-A459-4EA6-9FC7-DF620BE07CA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
CHARMS - Clinic Visits and Appointments
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/RASScenario2.xlsx
+++ b/src/test/java/CHARMS/resources/RASScenario2.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzipovay2/AquaProjects/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0CB48B-EE94-8744-85CA-B66B2B5102AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1262EF-5B91-BB4E-8570-6807806B3E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5860" yWindow="2420" windowWidth="24380" windowHeight="13480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="screenerScenario2" sheetId="1" r:id="rId1"/>
     <sheet name="IIQScenario2" sheetId="5" r:id="rId2"/>
-    <sheet name="RASSurveyScenario2" sheetId="4" r:id="rId3"/>
+    <sheet name="NewAppointment" sheetId="6" r:id="rId3"/>
+    <sheet name="ClinicVisit" sheetId="7" r:id="rId4"/>
+    <sheet name="RASSurveyScenario2" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3415" uniqueCount="3146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3477" uniqueCount="3192">
   <si>
     <t>Question</t>
   </si>
@@ -9636,6 +9638,144 @@
   </si>
   <si>
     <t>Do you currently live in the United States?</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Study</t>
+  </si>
+  <si>
+    <t>Appointment</t>
+  </si>
+  <si>
+    <t>Durations (hours)</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Provider</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Report Status</t>
+  </si>
+  <si>
+    <t>Scheduled Date/Time</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Test note</t>
+  </si>
+  <si>
+    <t>RASopathy</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>Test Provider</t>
+  </si>
+  <si>
+    <t>Scheduled</t>
+  </si>
+  <si>
+    <t>Other (Specify)</t>
+  </si>
+  <si>
+    <t>Other Report Status (Specify)</t>
+  </si>
+  <si>
+    <t>Report status test</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>Other (specify)</t>
+  </si>
+  <si>
+    <t>Other Appointment (Specify)</t>
+  </si>
+  <si>
+    <t>Other appointment test</t>
+  </si>
+  <si>
+    <t>Other Location (Specify)</t>
+  </si>
+  <si>
+    <t>Other location test</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Visit Type</t>
+  </si>
+  <si>
+    <t>Clinic Date</t>
+  </si>
+  <si>
+    <t>Primary Provider</t>
+  </si>
+  <si>
+    <t>Scheduling Coordinator</t>
+  </si>
+  <si>
+    <t>Preclinic Note Complete</t>
+  </si>
+  <si>
+    <t>Coordination with Other NIH Protocol</t>
+  </si>
+  <si>
+    <t>CRIS Order Status</t>
+  </si>
+  <si>
+    <t>Scheduling Status</t>
+  </si>
+  <si>
+    <t>After Hours Emergency Contact Name</t>
+  </si>
+  <si>
+    <t>After Hours Emergency Contact Number</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>Appointment Made</t>
+  </si>
+  <si>
+    <t>Lauren Black</t>
+  </si>
+  <si>
+    <t>Hodalis Gaytan</t>
+  </si>
+  <si>
+    <t>Specify NIH Protocol/Specialty</t>
+  </si>
+  <si>
+    <t>NIH protcol test</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Test Contact</t>
+  </si>
+  <si>
+    <t>Status Date</t>
+  </si>
+  <si>
+    <t>ScreenerTwoFirst T ScreenerTwoLast</t>
+  </si>
+  <si>
+    <t>04/02/1990</t>
   </si>
 </sst>
 </file>
@@ -9745,7 +9885,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -9810,6 +9950,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10129,8 +10276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11171,8 +11318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB9B37E-A256-1E4F-9B35-9A6E20F6FDB7}">
   <dimension ref="A1:B207"/>
   <sheetViews>
-    <sheetView topLeftCell="A359" workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12845,10 +12992,299 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4588FF6F-A8EF-054D-B3B4-987B41B9B6EE}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
+        <v>3146</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>3190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="26" t="s">
+        <v>3147</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>3157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
+        <v>3148</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>3165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
+        <v>3166</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>3167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
+        <v>3149</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>3158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="26" t="s">
+        <v>3150</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>3161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
+        <v>3168</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>3169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
+        <v>3151</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>3159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
+        <v>3152</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>3160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
+        <v>3189</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>3164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="26" t="s">
+        <v>3153</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>3161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
+        <v>3162</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>3163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="26" t="s">
+        <v>3154</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>3164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="26" t="s">
+        <v>3155</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>3156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B6" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6062CACA-7DB6-F649-B34B-70D7904C31B5}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3146</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>3190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3170</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>3191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3147</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>3157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3171</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>3181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3152</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>3182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3172</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>3164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3173</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>3183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3174</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>3184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3175</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3176</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>3185</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>3186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>3177</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>3187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>3178</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>3187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>3179</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>3188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>3180</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9D8CBE7-FBBE-194B-88E2-C1DC4C20EF1C}">
   <dimension ref="A1:B1412"/>
   <sheetViews>
-    <sheetView topLeftCell="A1226" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A1326" sqref="A1326"/>
     </sheetView>
   </sheetViews>
@@ -24139,6 +24575,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010084299BAE6AB37648AD80DEB59DC34125" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3eadf2c1f25cd7b71915c87a24a5e490">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="70b45aa3-433c-4bb7-a757-4861a21b7bcd" xmlns:ns3="f9acbf48-ccda-47b6-abb6-c9eb96c9ba33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="383f12c7747b491aea3350ad3b69b32a" ns2:_="" ns3:_="">
     <xsd:import namespace="70b45aa3-433c-4bb7-a757-4861a21b7bcd"/>
@@ -24309,22 +24760,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B75DB3A7-FCD6-4DD2-8F1A-F1A891316494}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A376A26F-A459-4EA6-9FC7-DF620BE07CA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8739BBC0-A319-48B2-92BB-329AC3208E3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24341,21 +24794,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B75DB3A7-FCD6-4DD2-8F1A-F1A891316494}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A376A26F-A459-4EA6-9FC7-DF620BE07CA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
CHARMS - Subject Flags
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/RASScenario2.xlsx
+++ b/src/test/java/CHARMS/resources/RASScenario2.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzipovay2/AquaProjects/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E308097-AC41-1742-BC34-C9286474AAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED0BED2-15DF-854E-9E5B-AF25F9E40EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5540" yWindow="10060" windowWidth="30240" windowHeight="17580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="screenerScenario2" sheetId="1" r:id="rId1"/>
-    <sheet name="IIQScenario2" sheetId="5" r:id="rId2"/>
-    <sheet name="NewAppointment" sheetId="6" r:id="rId3"/>
-    <sheet name="ClinicVisit" sheetId="7" r:id="rId4"/>
-    <sheet name="RASSurveyScenario2" sheetId="4" r:id="rId5"/>
+    <sheet name="SubjectFlags" sheetId="8" r:id="rId2"/>
+    <sheet name="IIQScenario2" sheetId="5" r:id="rId3"/>
+    <sheet name="NewAppointment" sheetId="6" r:id="rId4"/>
+    <sheet name="ClinicVisit" sheetId="7" r:id="rId5"/>
+    <sheet name="RASSurveyScenario2" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3489" uniqueCount="3208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3501" uniqueCount="3219">
   <si>
     <t>Question</t>
   </si>
@@ -9824,6 +9825,39 @@
   </si>
   <si>
     <t>Please complete the box below by selecting which primary cancers were diagnosed and at what age and year they occurred. If cancer spread from one place to another, please only indicate the original cancers and not the number of sites where cancer spread. Year of diagnosis Option 4</t>
+  </si>
+  <si>
+    <t>Participation Status</t>
+  </si>
+  <si>
+    <t>Eligible for Clinic</t>
+  </si>
+  <si>
+    <t>Individual Affected Status</t>
+  </si>
+  <si>
+    <t>Individual Genetic Status</t>
+  </si>
+  <si>
+    <t>Family Genetic Status</t>
+  </si>
+  <si>
+    <t>Eligible to Participate</t>
+  </si>
+  <si>
+    <t>Clinically Affected</t>
+  </si>
+  <si>
+    <t>Variant Positive</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Subject Comments</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -10324,7 +10358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
@@ -11443,6 +11477,71 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F400B75-2DF6-0441-8E77-101DA5DAEA4D}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3208</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3209</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3210</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3211</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3212</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3217</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3218</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB9B37E-A256-1E4F-9B35-9A6E20F6FDB7}">
   <dimension ref="A1:B207"/>
   <sheetViews>
@@ -11978,7 +12077,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="s">
         <v>3008</v>
       </c>
@@ -11994,7 +12093,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="19" t="s">
         <v>3006</v>
       </c>
@@ -13119,7 +13218,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4588FF6F-A8EF-054D-B3B4-987B41B9B6EE}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -13261,7 +13360,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6062CACA-7DB6-F649-B34B-70D7904C31B5}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -13408,7 +13507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9D8CBE7-FBBE-194B-88E2-C1DC4C20EF1C}">
   <dimension ref="A1:B1412"/>
   <sheetViews>
@@ -24703,6 +24802,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010084299BAE6AB37648AD80DEB59DC34125" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3eadf2c1f25cd7b71915c87a24a5e490">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="70b45aa3-433c-4bb7-a757-4861a21b7bcd" xmlns:ns3="f9acbf48-ccda-47b6-abb6-c9eb96c9ba33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="383f12c7747b491aea3350ad3b69b32a" ns2:_="" ns3:_="">
     <xsd:import namespace="70b45aa3-433c-4bb7-a757-4861a21b7bcd"/>
@@ -24873,22 +24987,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B75DB3A7-FCD6-4DD2-8F1A-F1A891316494}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A376A26F-A459-4EA6-9FC7-DF620BE07CA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8739BBC0-A319-48B2-92BB-329AC3208E3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24905,21 +25021,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A376A26F-A459-4EA6-9FC7-DF620BE07CA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B75DB3A7-FCD6-4DD2-8F1A-F1A891316494}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
CHARMS - Post-Clinic automation plus updates to QBank tests
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/RASScenario2.xlsx
+++ b/src/test/java/CHARMS/resources/RASScenario2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzipovay2/AquaProjects/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764242BE-0794-5740-B9BC-DE29721DC27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFABE5E-5583-F14B-BFE8-554ADD0EAEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="screenerScenario2" sheetId="1" r:id="rId1"/>
@@ -10526,8 +10526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B163"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11727,8 +11727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68E42E2-294A-9347-A83B-FE2A03CE7613}">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12614,7 +12614,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="s">
         <v>3008</v>
       </c>
@@ -12630,7 +12630,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" s="19" t="s">
         <v>3006</v>
       </c>
@@ -25339,21 +25339,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010084299BAE6AB37648AD80DEB59DC34125" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3eadf2c1f25cd7b71915c87a24a5e490">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="70b45aa3-433c-4bb7-a757-4861a21b7bcd" xmlns:ns3="f9acbf48-ccda-47b6-abb6-c9eb96c9ba33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="383f12c7747b491aea3350ad3b69b32a" ns2:_="" ns3:_="">
     <xsd:import namespace="70b45aa3-433c-4bb7-a757-4861a21b7bcd"/>
@@ -25524,24 +25509,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A376A26F-A459-4EA6-9FC7-DF620BE07CA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B75DB3A7-FCD6-4DD2-8F1A-F1A891316494}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8739BBC0-A319-48B2-92BB-329AC3208E3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25558,4 +25541,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B75DB3A7-FCD6-4DD2-8F1A-F1A891316494}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A376A26F-A459-4EA6-9FC7-DF620BE07CA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>